<commit_message>
ES Works Start Datagen Connector
</commit_message>
<xml_diff>
--- a/doc/Operators.xlsx
+++ b/doc/Operators.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CurrentProjects\CP4I\Installation\cp4i-install\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C3A16B03-98E9-4182-80F3-567971B87EE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F8FFF9D-F61D-41A4-BB55-C0A620F3E89D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="64065" yWindow="1440" windowWidth="24840" windowHeight="15990" xr2:uid="{7EC31224-7A59-4758-9982-0385BBCD6FB8}"/>
+    <workbookView xWindow="57480" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{7EC31224-7A59-4758-9982-0385BBCD6FB8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$2:$M$17</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -36,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="75">
   <si>
     <t>cert-manager-operator</t>
   </si>
@@ -121,47 +124,200 @@
     <t>Provided APIs</t>
   </si>
   <si>
-    <t>cert-manager Operator for Red Hat OpenShift 1.12.1 (Red Hat)</t>
-  </si>
-  <si>
-    <t>IBM DataPower Gateway 1.9.0 (IBM)</t>
-  </si>
-  <si>
-    <t>IBM API Connect 5.1.0 (IBM)</t>
-  </si>
-  <si>
-    <t>IBM Cloud Pak foundational services 4.3.1 (IBM)</t>
-  </si>
-  <si>
-    <t>IBM Event Streams 3.3.1 (IBM)</t>
-  </si>
-  <si>
-    <t>IBM Licensing 4.2.2 (IBM)</t>
-  </si>
-  <si>
-    <t>IBM MQ 3.0.1 (IBM)</t>
-  </si>
-  <si>
-    <t>Local Storage 4.14.0-202404161544 (Red Hat)</t>
-  </si>
-  <si>
-    <t>OpenShift Data Foundation 4.14.6-rhodf (Red Hat)</t>
-  </si>
-  <si>
-    <t>Operand Deployment Lifecycle Manager 4.2.2 (IBM)</t>
-  </si>
-  <si>
-    <t>Package Server 0.0.1-snapshot (Red Hat)</t>
-  </si>
-  <si>
     <t>Operator Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> CommonService</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Flink Deployment</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> EventProcessing</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Queue Manager</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> cert-manager-operator</t>
+  </si>
+  <si>
+    <t xml:space="preserve">openshift-operators </t>
+  </si>
+  <si>
+    <t>CertificateRequest
+Certificate Challenge
+ClusterIssuer
+View 3 more…</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> DataPowerService
+DataPowerMonitor
+DataPowerMustGather
+DataPowerMustGatherManager</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Analytics backup task
+Analytics cluster
+Analytics restore task
+API Connect cluster
+View 9 more...</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Event Endpoint Management
+Event Gateway</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Event Streams
+Kafka Connect
+Kafka Topic
+Kafka User
+View 5 more...</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Platform UI
+Integration assembly
+Declarative API
+Declarative API Product</t>
+  </si>
+  <si>
+    <t>Local Volume Local
+Volume Set Local
+Volume Discovery</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> OperandBindInfo
+OperandConfig
+OperandRegistry
+OperandRequest</t>
+  </si>
+  <si>
+    <t>cert-manager Operator for Red Hat OpenShift</t>
+  </si>
+  <si>
+    <t>1.13.0</t>
+  </si>
+  <si>
+    <t>(Red Hat)</t>
+  </si>
+  <si>
+    <t>IBM DataPower Gateway</t>
+  </si>
+  <si>
+    <t>1.9.1</t>
+  </si>
+  <si>
+    <t>(IBM)</t>
+  </si>
+  <si>
+    <t>IBM API Connect</t>
+  </si>
+  <si>
+    <t>5.1.0</t>
+  </si>
+  <si>
+    <t>IBM Cloud Pak foundational services</t>
+  </si>
+  <si>
+    <t>4.5.0</t>
+  </si>
+  <si>
+    <t>IBM Operator for Apache Flink</t>
+  </si>
+  <si>
+    <t>1.1.4</t>
+  </si>
+  <si>
+    <t>IBM Event Endpoint Management</t>
+  </si>
+  <si>
+    <t>11.1.4</t>
+  </si>
+  <si>
+    <t>IBM Event Processing</t>
+  </si>
+  <si>
+    <t>IBM Event Streams</t>
+  </si>
+  <si>
+    <t>3.3.1</t>
+  </si>
+  <si>
+    <t>IBM Cloud Pak for Integration</t>
+  </si>
+  <si>
+    <t>7.2.4</t>
+  </si>
+  <si>
+    <t>IBM MQ</t>
+  </si>
+  <si>
+    <t>3.1.2</t>
+  </si>
+  <si>
+    <t>4.14.0-202404161544</t>
+  </si>
+  <si>
+    <t>OpenShift Data Foundation</t>
+  </si>
+  <si>
+    <t>4.14.6-rhodf</t>
+  </si>
+  <si>
+    <t>Operand Deployment Lifecycle Manager</t>
+  </si>
+  <si>
+    <t>4.2.3</t>
+  </si>
+  <si>
+    <t>IBM Licensing</t>
+  </si>
+  <si>
+    <t>4.2.2</t>
+  </si>
+  <si>
+    <t>Local Storage</t>
+  </si>
+  <si>
+    <t>Package Server</t>
+  </si>
+  <si>
+    <t>0.0.1-snapshot</t>
+  </si>
+  <si>
+    <t>Version</t>
+  </si>
+  <si>
+    <t>Provider</t>
+  </si>
+  <si>
+    <t>Saad - Arnauld - TechZone</t>
+  </si>
+  <si>
+    <t>EDA - TechZone</t>
+  </si>
+  <si>
+    <t>Keycloak Operator</t>
+  </si>
+  <si>
+    <t>22.0.10-opr.1</t>
+  </si>
+  <si>
+    <t>ibm-common-services</t>
+  </si>
+  <si>
+    <t>KeycloakRealm
+Import Keycloak</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="8" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -173,6 +329,13 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -198,12 +361,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -538,188 +706,659 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90B01659-04B3-4430-BFC1-4B57B6835BA3}">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:M20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="51.3671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="32.05078125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.62890625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="37.83984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.41796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.05078125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="32.05078125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.62890625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="37.83984375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.41796875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.05078125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.3125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="21.89453125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="26.62890625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="H1" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="72" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H3" t="s">
+        <v>36</v>
+      </c>
+      <c r="I3" t="s">
+        <v>37</v>
+      </c>
+      <c r="J3" t="s">
+        <v>38</v>
+      </c>
+      <c r="K3" t="s">
+        <v>0</v>
+      </c>
+      <c r="L3" t="s">
+        <v>26</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" t="s">
+        <v>39</v>
+      </c>
+      <c r="I4" t="s">
+        <v>40</v>
+      </c>
+      <c r="J4" t="s">
+        <v>41</v>
+      </c>
+      <c r="K4" t="s">
+        <v>27</v>
+      </c>
+      <c r="L4" t="s">
+        <v>3</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="72" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H5" t="s">
+        <v>42</v>
+      </c>
+      <c r="I5" t="s">
+        <v>43</v>
+      </c>
+      <c r="J5" t="s">
+        <v>41</v>
+      </c>
+      <c r="K5" t="s">
+        <v>27</v>
+      </c>
+      <c r="L5" t="s">
+        <v>3</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C6" t="s">
+        <v>41</v>
+      </c>
+      <c r="D6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F6" t="s">
+        <v>4</v>
+      </c>
+      <c r="H6" t="s">
+        <v>44</v>
+      </c>
+      <c r="I6" t="s">
+        <v>45</v>
+      </c>
+      <c r="J6" t="s">
+        <v>41</v>
+      </c>
+      <c r="K6" t="s">
+        <v>27</v>
+      </c>
+      <c r="L6" t="s">
+        <v>3</v>
+      </c>
+      <c r="M6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" t="s">
+        <v>46</v>
+      </c>
+      <c r="B7" t="s">
+        <v>47</v>
+      </c>
+      <c r="C7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" t="s">
+        <v>3</v>
+      </c>
+      <c r="F7" t="s">
+        <v>23</v>
+      </c>
+      <c r="H7" t="s">
+        <v>46</v>
+      </c>
+      <c r="I7" t="s">
+        <v>47</v>
+      </c>
+      <c r="J7" t="s">
+        <v>41</v>
+      </c>
+      <c r="K7" t="s">
+        <v>27</v>
+      </c>
+      <c r="L7" t="s">
+        <v>3</v>
+      </c>
+      <c r="M7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" t="s">
+        <v>48</v>
+      </c>
+      <c r="B8" t="s">
+        <v>49</v>
+      </c>
+      <c r="C8" t="s">
+        <v>41</v>
+      </c>
+      <c r="D8" t="s">
+        <v>27</v>
+      </c>
+      <c r="E8" t="s">
+        <v>3</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H8" t="s">
+        <v>48</v>
+      </c>
+      <c r="I8" t="s">
+        <v>49</v>
+      </c>
+      <c r="J8" t="s">
+        <v>41</v>
+      </c>
+      <c r="K8" t="s">
+        <v>27</v>
+      </c>
+      <c r="L8" t="s">
+        <v>3</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" t="s">
+        <v>50</v>
+      </c>
+      <c r="B9" t="s">
+        <v>47</v>
+      </c>
+      <c r="C9" t="s">
+        <v>41</v>
+      </c>
+      <c r="D9" t="s">
+        <v>27</v>
+      </c>
+      <c r="E9" t="s">
+        <v>3</v>
+      </c>
+      <c r="F9" t="s">
+        <v>24</v>
+      </c>
+      <c r="H9" t="s">
+        <v>50</v>
+      </c>
+      <c r="I9" t="s">
+        <v>47</v>
+      </c>
+      <c r="J9" t="s">
+        <v>41</v>
+      </c>
+      <c r="K9" t="s">
+        <v>27</v>
+      </c>
+      <c r="L9" t="s">
+        <v>3</v>
+      </c>
+      <c r="M9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="72" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" t="s">
+        <v>51</v>
+      </c>
+      <c r="B10" t="s">
+        <v>52</v>
+      </c>
+      <c r="C10" t="s">
+        <v>41</v>
+      </c>
+      <c r="D10" t="s">
+        <v>2</v>
+      </c>
+      <c r="E10" t="s">
+        <v>3</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H10" t="s">
+        <v>51</v>
+      </c>
+      <c r="I10" t="s">
+        <v>52</v>
+      </c>
+      <c r="J10" t="s">
+        <v>41</v>
+      </c>
+      <c r="K10" t="s">
+        <v>27</v>
+      </c>
+      <c r="L10" t="s">
+        <v>3</v>
+      </c>
+      <c r="M10" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="72" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="57.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B3" t="s">
+    </row>
+    <row r="11" spans="1:13" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" t="s">
+        <v>53</v>
+      </c>
+      <c r="B11" t="s">
+        <v>54</v>
+      </c>
+      <c r="C11" t="s">
+        <v>41</v>
+      </c>
+      <c r="F11" s="1"/>
+      <c r="H11" t="s">
+        <v>53</v>
+      </c>
+      <c r="I11" t="s">
+        <v>54</v>
+      </c>
+      <c r="J11" t="s">
+        <v>41</v>
+      </c>
+      <c r="K11" t="s">
+        <v>27</v>
+      </c>
+      <c r="L11" t="s">
+        <v>3</v>
+      </c>
+      <c r="M11" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B12" t="s">
+        <v>63</v>
+      </c>
+      <c r="C12" t="s">
+        <v>41</v>
+      </c>
+      <c r="D12" t="s">
+        <v>5</v>
+      </c>
+      <c r="E12" t="s">
+        <v>5</v>
+      </c>
+      <c r="F12" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" t="s">
+        <v>55</v>
+      </c>
+      <c r="B13" t="s">
+        <v>56</v>
+      </c>
+      <c r="C13" t="s">
+        <v>41</v>
+      </c>
+      <c r="D13" t="s">
         <v>2</v>
       </c>
-      <c r="C3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="72" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="E13" t="s">
+        <v>3</v>
+      </c>
+      <c r="F13" t="s">
+        <v>7</v>
+      </c>
+      <c r="H13" t="s">
+        <v>55</v>
+      </c>
+      <c r="I13" t="s">
+        <v>56</v>
+      </c>
+      <c r="J13" t="s">
+        <v>41</v>
+      </c>
+      <c r="K13" t="s">
+        <v>27</v>
+      </c>
+      <c r="L13" t="s">
+        <v>3</v>
+      </c>
+      <c r="M13" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" t="s">
+        <v>71</v>
+      </c>
+      <c r="B14" t="s">
+        <v>72</v>
+      </c>
+      <c r="C14" t="s">
+        <v>38</v>
+      </c>
+      <c r="D14" t="s">
+        <v>73</v>
+      </c>
+      <c r="E14" t="s">
+        <v>73</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="H14" t="s">
+        <v>71</v>
+      </c>
+      <c r="I14" t="s">
+        <v>72</v>
+      </c>
+      <c r="J14" t="s">
+        <v>38</v>
+      </c>
+      <c r="K14" t="s">
+        <v>73</v>
+      </c>
+      <c r="L14" t="s">
+        <v>73</v>
+      </c>
+      <c r="M14" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" t="s">
+        <v>64</v>
+      </c>
+      <c r="B15" t="s">
+        <v>57</v>
+      </c>
+      <c r="C15" t="s">
+        <v>38</v>
+      </c>
+      <c r="D15" t="s">
+        <v>8</v>
+      </c>
+      <c r="E15" t="s">
+        <v>8</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H15" t="s">
+        <v>64</v>
+      </c>
+      <c r="I15" t="s">
+        <v>57</v>
+      </c>
+      <c r="J15" t="s">
+        <v>38</v>
+      </c>
+      <c r="K15" t="s">
+        <v>8</v>
+      </c>
+      <c r="L15" t="s">
+        <v>8</v>
+      </c>
+      <c r="M15" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16" t="s">
+        <v>58</v>
+      </c>
+      <c r="B16" t="s">
+        <v>59</v>
+      </c>
+      <c r="C16" t="s">
+        <v>38</v>
+      </c>
+      <c r="D16" t="s">
+        <v>9</v>
+      </c>
+      <c r="E16" t="s">
+        <v>9</v>
+      </c>
+      <c r="F16" t="s">
+        <v>10</v>
+      </c>
+      <c r="H16" t="s">
+        <v>58</v>
+      </c>
+      <c r="I16" t="s">
+        <v>59</v>
+      </c>
+      <c r="J16" t="s">
+        <v>38</v>
+      </c>
+      <c r="K16" t="s">
+        <v>9</v>
+      </c>
+      <c r="L16" t="s">
+        <v>9</v>
+      </c>
+      <c r="M16" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17" t="s">
+        <v>60</v>
+      </c>
+      <c r="B17" t="s">
+        <v>61</v>
+      </c>
+      <c r="C17" t="s">
+        <v>41</v>
+      </c>
+      <c r="D17" t="s">
         <v>2</v>
       </c>
-      <c r="C4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" t="s">
-        <v>24</v>
-      </c>
-      <c r="B5" t="s">
-        <v>2</v>
-      </c>
-      <c r="C5" t="s">
-        <v>3</v>
-      </c>
-      <c r="D5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="72" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" t="s">
-        <v>25</v>
-      </c>
-      <c r="B6" t="s">
-        <v>2</v>
-      </c>
-      <c r="C6" t="s">
-        <v>3</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" t="s">
-        <v>26</v>
-      </c>
-      <c r="B7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" t="s">
-        <v>5</v>
-      </c>
-      <c r="D7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" t="s">
+      <c r="E17" t="s">
+        <v>3</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H17" t="s">
+        <v>60</v>
+      </c>
+      <c r="I17" t="s">
+        <v>61</v>
+      </c>
+      <c r="J17" t="s">
+        <v>41</v>
+      </c>
+      <c r="K17" t="s">
         <v>27</v>
       </c>
-      <c r="B8" t="s">
-        <v>2</v>
-      </c>
-      <c r="C8" t="s">
-        <v>3</v>
-      </c>
-      <c r="D8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" t="s">
-        <v>28</v>
-      </c>
-      <c r="B9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9" t="s">
-        <v>8</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" t="s">
-        <v>29</v>
-      </c>
-      <c r="B10" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" t="s">
-        <v>9</v>
-      </c>
-      <c r="D10" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="57.6" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" t="s">
-        <v>30</v>
-      </c>
-      <c r="B11" t="s">
-        <v>2</v>
-      </c>
-      <c r="C11" t="s">
-        <v>3</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12" t="s">
-        <v>31</v>
-      </c>
-      <c r="B12" t="s">
+      <c r="L17" t="s">
+        <v>3</v>
+      </c>
+      <c r="M17" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B18" t="s">
+        <v>66</v>
+      </c>
+      <c r="C18" t="s">
+        <v>38</v>
+      </c>
+      <c r="D18" t="s">
         <v>11</v>
       </c>
-      <c r="C12" t="s">
+      <c r="E18" t="s">
         <v>11</v>
       </c>
-      <c r="D12" t="s">
+      <c r="F18" t="s">
         <v>12</v>
       </c>
     </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="H19" s="5"/>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="H20" s="5"/>
+    </row>
   </sheetData>
+  <autoFilter ref="A2:M17" xr:uid="{90B01659-04B3-4430-BFC1-4B57B6835BA3}"/>
+  <mergeCells count="2">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="H1:M1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>